<commit_message>
Found more Taylor-coded data. Bless her.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/digits_TG.xlsx
+++ b/raw-data-prep/raw_data/digits_TG.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Subno</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>crooked finger, little unclear</t>
+  </si>
+  <si>
+    <t>Fingers kinda crooked</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -396,11 +402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J137"/>
+  <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J138" sqref="J138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,310 +2615,1833 @@
       <c r="A76">
         <v>246</v>
       </c>
+      <c r="B76">
+        <v>867.4</v>
+      </c>
+      <c r="C76">
+        <v>86.7</v>
+      </c>
+      <c r="D76">
+        <v>809.4</v>
+      </c>
+      <c r="E76">
+        <v>84.75</v>
+      </c>
+      <c r="F76">
+        <v>812.6</v>
+      </c>
+      <c r="G76">
+        <v>81.650000000000006</v>
+      </c>
+      <c r="H76">
+        <v>828.2</v>
+      </c>
+      <c r="I76">
+        <v>88.75</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>247</v>
       </c>
+      <c r="B77">
+        <v>898.2</v>
+      </c>
+      <c r="C77">
+        <v>88.85</v>
+      </c>
+      <c r="D77">
+        <v>888.2</v>
+      </c>
+      <c r="E77">
+        <v>74.52</v>
+      </c>
+      <c r="F77">
+        <v>873.9</v>
+      </c>
+      <c r="G77">
+        <v>76.3</v>
+      </c>
+      <c r="H77">
+        <v>895</v>
+      </c>
+      <c r="I77">
+        <v>87.31</v>
+      </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>248</v>
       </c>
+      <c r="B78">
+        <v>874.9</v>
+      </c>
+      <c r="C78">
+        <v>87.45</v>
+      </c>
+      <c r="D78">
+        <v>819.8</v>
+      </c>
+      <c r="E78">
+        <v>83.2</v>
+      </c>
+      <c r="F78">
+        <v>838.1</v>
+      </c>
+      <c r="G78">
+        <v>87.13</v>
+      </c>
+      <c r="H78">
+        <v>872.4</v>
+      </c>
+      <c r="I78">
+        <v>84.94</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>249</v>
       </c>
+      <c r="B79">
+        <v>1019.2</v>
+      </c>
+      <c r="C79">
+        <v>82.73</v>
+      </c>
+      <c r="D79">
+        <v>904.6</v>
+      </c>
+      <c r="E79">
+        <v>86.58</v>
+      </c>
+      <c r="F79">
+        <v>922.7</v>
+      </c>
+      <c r="G79">
+        <v>86.52</v>
+      </c>
+      <c r="H79">
+        <v>1035.4000000000001</v>
+      </c>
+      <c r="I79">
+        <v>82.68</v>
+      </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>250</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80">
+        <v>928.5</v>
+      </c>
+      <c r="C80">
+        <v>84.38</v>
+      </c>
+      <c r="D80">
+        <v>838.6</v>
+      </c>
+      <c r="E80">
+        <v>87.74</v>
+      </c>
+      <c r="F80">
+        <v>834.7</v>
+      </c>
+      <c r="G80">
+        <v>87.67</v>
+      </c>
+      <c r="H80">
+        <v>888.9</v>
+      </c>
+      <c r="I80">
+        <v>83.41</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>251</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>953.7</v>
+      </c>
+      <c r="C81">
+        <v>86.57</v>
+      </c>
+      <c r="D81">
+        <v>918.3</v>
+      </c>
+      <c r="E81">
+        <v>88.5</v>
+      </c>
+      <c r="F81">
+        <v>925.1</v>
+      </c>
+      <c r="G81">
+        <v>87.15</v>
+      </c>
+      <c r="H81">
+        <v>933.3</v>
+      </c>
+      <c r="I81">
+        <v>88.53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>252</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>889.5</v>
+      </c>
+      <c r="C82">
+        <v>84.26</v>
+      </c>
+      <c r="D82">
+        <v>858.1</v>
+      </c>
+      <c r="E82">
+        <v>87.13</v>
+      </c>
+      <c r="F82">
+        <v>848.4</v>
+      </c>
+      <c r="G82">
+        <v>88.18</v>
+      </c>
+      <c r="H82">
+        <v>902.7</v>
+      </c>
+      <c r="I82">
+        <v>81.59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>253</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>958.2</v>
+      </c>
+      <c r="C83">
+        <v>84.61</v>
+      </c>
+      <c r="D83">
+        <v>929.8</v>
+      </c>
+      <c r="E83">
+        <v>84.82</v>
+      </c>
+      <c r="F83">
+        <v>913.8</v>
+      </c>
+      <c r="G83">
+        <v>83.02</v>
+      </c>
+      <c r="H83">
+        <v>961.2</v>
+      </c>
+      <c r="I83">
+        <v>88.75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>254</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84">
+        <v>1005.5</v>
+      </c>
+      <c r="C84">
+        <v>86.92</v>
+      </c>
+      <c r="D84">
+        <v>969.7</v>
+      </c>
+      <c r="E84">
+        <v>87.87</v>
+      </c>
+      <c r="F84">
+        <v>946.8</v>
+      </c>
+      <c r="G84">
+        <v>86.43</v>
+      </c>
+      <c r="H84">
+        <v>992.5</v>
+      </c>
+      <c r="I84">
+        <v>88.09</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>255</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>897.2</v>
+      </c>
+      <c r="C85">
+        <v>88.66</v>
+      </c>
+      <c r="D85">
+        <v>843.6</v>
+      </c>
+      <c r="E85">
+        <v>83.4</v>
+      </c>
+      <c r="F85">
+        <v>845.4</v>
+      </c>
+      <c r="G85">
+        <v>85.73</v>
+      </c>
+      <c r="H85">
+        <v>884.1</v>
+      </c>
+      <c r="I85">
+        <v>89.03</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>256</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>935.7</v>
+      </c>
+      <c r="C86">
+        <v>86.57</v>
+      </c>
+      <c r="D86">
+        <v>886.2</v>
+      </c>
+      <c r="E86">
+        <v>85.99</v>
+      </c>
+      <c r="F86">
+        <v>908.9</v>
+      </c>
+      <c r="G86">
+        <v>84.06</v>
+      </c>
+      <c r="H86">
+        <v>923.6</v>
+      </c>
+      <c r="I86">
+        <v>88.01</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>257</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>817.2</v>
+      </c>
+      <c r="C87">
+        <v>84.95</v>
+      </c>
+      <c r="D87">
+        <v>803.8</v>
+      </c>
+      <c r="E87">
+        <v>86.15</v>
+      </c>
+      <c r="F87">
+        <v>786.5</v>
+      </c>
+      <c r="G87">
+        <v>83.87</v>
+      </c>
+      <c r="H87">
+        <v>819.7</v>
+      </c>
+      <c r="I87">
+        <v>86.36</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>258</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <v>846.2</v>
+      </c>
+      <c r="C88">
+        <v>84.3</v>
+      </c>
+      <c r="D88">
+        <v>882.2</v>
+      </c>
+      <c r="E88">
+        <v>88.83</v>
+      </c>
+      <c r="F88">
+        <v>859.6</v>
+      </c>
+      <c r="G88">
+        <v>87.8</v>
+      </c>
+      <c r="H88">
+        <v>864</v>
+      </c>
+      <c r="I88">
+        <v>87.21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>259</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>983.5</v>
+      </c>
+      <c r="C89">
+        <v>81.23</v>
+      </c>
+      <c r="D89">
+        <v>902.8</v>
+      </c>
+      <c r="E89">
+        <v>87.59</v>
+      </c>
+      <c r="F89">
+        <v>887.3</v>
+      </c>
+      <c r="G89">
+        <v>85.09</v>
+      </c>
+      <c r="H89">
+        <v>999.2</v>
+      </c>
+      <c r="I89">
+        <v>87.25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>260</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90">
+        <v>914.2</v>
+      </c>
+      <c r="C90">
+        <v>85.99</v>
+      </c>
+      <c r="D90">
+        <v>876.3</v>
+      </c>
+      <c r="E90">
+        <v>88.56</v>
+      </c>
+      <c r="F90">
+        <v>880.8</v>
+      </c>
+      <c r="G90">
+        <v>87.53</v>
+      </c>
+      <c r="H90">
+        <v>909</v>
+      </c>
+      <c r="I90">
+        <v>87.35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>261</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91">
+        <v>903.4</v>
+      </c>
+      <c r="C91">
+        <v>88.29</v>
+      </c>
+      <c r="D91">
+        <v>861.2</v>
+      </c>
+      <c r="E91">
+        <v>85.07</v>
+      </c>
+      <c r="F91">
+        <v>843.9</v>
+      </c>
+      <c r="G91">
+        <v>87.28</v>
+      </c>
+      <c r="H91">
+        <v>895.8</v>
+      </c>
+      <c r="I91">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>262</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>930.8</v>
+      </c>
+      <c r="C92">
+        <v>87.66</v>
+      </c>
+      <c r="D92">
+        <v>878.4</v>
+      </c>
+      <c r="E92">
+        <v>83.07</v>
+      </c>
+      <c r="F92">
+        <v>906.3</v>
+      </c>
+      <c r="G92">
+        <v>81.37</v>
+      </c>
+      <c r="H92">
+        <v>932</v>
+      </c>
+      <c r="I92">
+        <v>89.63</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>263</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>840.9</v>
+      </c>
+      <c r="C93">
+        <v>85.23</v>
+      </c>
+      <c r="D93">
+        <v>838.7</v>
+      </c>
+      <c r="E93">
+        <v>86.31</v>
+      </c>
+      <c r="F93">
+        <v>825.3</v>
+      </c>
+      <c r="G93">
+        <v>82.9</v>
+      </c>
+      <c r="H93">
+        <v>967.4</v>
+      </c>
+      <c r="I93">
+        <v>88.35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>264</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>884</v>
+      </c>
+      <c r="C94">
+        <v>89.48</v>
+      </c>
+      <c r="D94">
+        <v>778.5</v>
+      </c>
+      <c r="E94">
+        <v>85.43</v>
+      </c>
+      <c r="F94">
+        <v>800.8</v>
+      </c>
+      <c r="G94">
+        <v>87.42</v>
+      </c>
+      <c r="H94">
+        <v>883.4</v>
+      </c>
+      <c r="I94">
+        <v>86.76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>265</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <v>888</v>
+      </c>
+      <c r="C95">
+        <v>89.42</v>
+      </c>
+      <c r="D95">
+        <v>843.6</v>
+      </c>
+      <c r="E95">
+        <v>82.85</v>
+      </c>
+      <c r="F95">
+        <v>837.2</v>
+      </c>
+      <c r="G95">
+        <v>77.37</v>
+      </c>
+      <c r="H95">
+        <v>900.2</v>
+      </c>
+      <c r="I95">
+        <v>88.79</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>266</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96">
+        <v>996.3</v>
+      </c>
+      <c r="C96">
+        <v>88.62</v>
+      </c>
+      <c r="D96">
+        <v>1000.2</v>
+      </c>
+      <c r="E96">
+        <v>88.97</v>
+      </c>
+      <c r="F96">
+        <v>1013.7</v>
+      </c>
+      <c r="G96">
+        <v>85.13</v>
+      </c>
+      <c r="H96">
+        <v>990</v>
+      </c>
+      <c r="I96">
+        <v>89.54</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>267</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>912.1</v>
+      </c>
+      <c r="C97">
+        <v>89.37</v>
+      </c>
+      <c r="D97">
+        <v>859.4</v>
+      </c>
+      <c r="E97">
+        <v>79.13</v>
+      </c>
+      <c r="F97">
+        <v>877.1</v>
+      </c>
+      <c r="G97">
+        <v>81.739999999999995</v>
+      </c>
+      <c r="H97">
+        <v>918.2</v>
+      </c>
+      <c r="I97">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>268</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98">
+        <v>909.7</v>
+      </c>
+      <c r="C98">
+        <v>82.55</v>
+      </c>
+      <c r="D98">
+        <v>880</v>
+      </c>
+      <c r="E98">
+        <v>89.61</v>
+      </c>
+      <c r="F98">
+        <v>882</v>
+      </c>
+      <c r="G98">
+        <v>89.87</v>
+      </c>
+      <c r="H98">
+        <v>887.4</v>
+      </c>
+      <c r="I98">
+        <v>84.86</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>269</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>968.6</v>
+      </c>
+      <c r="C99">
+        <v>84.43</v>
+      </c>
+      <c r="D99">
+        <v>889.5</v>
+      </c>
+      <c r="E99">
+        <v>86.65</v>
+      </c>
+      <c r="F99">
+        <v>911.2</v>
+      </c>
+      <c r="G99">
+        <v>82.81</v>
+      </c>
+      <c r="H99">
+        <v>979.2</v>
+      </c>
+      <c r="I99">
+        <v>81.31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>270</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100">
+        <v>967.4</v>
+      </c>
+      <c r="C100">
+        <v>86.92</v>
+      </c>
+      <c r="D100">
+        <v>935.4</v>
+      </c>
+      <c r="E100">
+        <v>86.81</v>
+      </c>
+      <c r="F100">
+        <v>937.1</v>
+      </c>
+      <c r="G100">
+        <v>87.19</v>
+      </c>
+      <c r="H100">
+        <v>958.4</v>
+      </c>
+      <c r="I100">
+        <v>88.33</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>271</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101">
+        <v>831.7</v>
+      </c>
+      <c r="C101">
+        <v>75.16</v>
+      </c>
+      <c r="D101">
+        <v>854.8</v>
+      </c>
+      <c r="E101">
+        <v>85.37</v>
+      </c>
+      <c r="F101">
+        <v>840.6</v>
+      </c>
+      <c r="G101">
+        <v>84.68</v>
+      </c>
+      <c r="H101">
+        <v>816.8</v>
+      </c>
+      <c r="I101">
+        <v>78.349999999999994</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>272</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102">
+        <v>921.1</v>
+      </c>
+      <c r="C102">
+        <v>89.32</v>
+      </c>
+      <c r="D102">
+        <v>866</v>
+      </c>
+      <c r="E102">
+        <v>83.84</v>
+      </c>
+      <c r="F102">
+        <v>871.2</v>
+      </c>
+      <c r="G102">
+        <v>87.04</v>
+      </c>
+      <c r="H102">
+        <v>911.1</v>
+      </c>
+      <c r="I102">
+        <v>85.28</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>273</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103">
+        <v>792</v>
+      </c>
+      <c r="C103">
+        <v>77.09</v>
+      </c>
+      <c r="D103">
+        <v>794.5</v>
+      </c>
+      <c r="E103">
+        <v>83.93</v>
+      </c>
+      <c r="F103">
+        <v>801.2</v>
+      </c>
+      <c r="G103">
+        <v>81.31</v>
+      </c>
+      <c r="H103">
+        <v>822.7</v>
+      </c>
+      <c r="I103">
+        <v>75.930000000000007</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>274</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104">
+        <v>1032</v>
+      </c>
+      <c r="C104">
+        <v>86.44</v>
+      </c>
+      <c r="D104">
+        <v>996.8</v>
+      </c>
+      <c r="E104">
+        <v>87.7</v>
+      </c>
+      <c r="F104">
+        <v>986.2</v>
+      </c>
+      <c r="G104">
+        <v>88.95</v>
+      </c>
+      <c r="H104">
+        <v>1031.0999999999999</v>
+      </c>
+      <c r="I104">
+        <v>84.32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>275</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>865.5</v>
+      </c>
+      <c r="C105">
+        <v>79.88</v>
+      </c>
+      <c r="D105">
+        <v>865.2</v>
+      </c>
+      <c r="E105">
+        <v>85.09</v>
+      </c>
+      <c r="F105">
+        <v>862.1</v>
+      </c>
+      <c r="G105">
+        <v>89.2</v>
+      </c>
+      <c r="H105">
+        <v>866.5</v>
+      </c>
+      <c r="I105">
+        <v>82.97</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>276</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <v>930</v>
+      </c>
+      <c r="C106">
+        <v>89.88</v>
+      </c>
+      <c r="D106">
+        <v>872.2</v>
+      </c>
+      <c r="E106">
+        <v>84.34</v>
+      </c>
+      <c r="F106">
+        <v>876.8</v>
+      </c>
+      <c r="G106">
+        <v>83.98</v>
+      </c>
+      <c r="H106">
+        <v>942.1</v>
+      </c>
+      <c r="I106">
+        <v>89.03</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>277</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107">
+        <v>880.5</v>
+      </c>
+      <c r="C107">
+        <v>88.05</v>
+      </c>
+      <c r="D107">
+        <v>850.4</v>
+      </c>
+      <c r="E107">
+        <v>85.68</v>
+      </c>
+      <c r="F107">
+        <v>846.6</v>
+      </c>
+      <c r="G107">
+        <v>85.53</v>
+      </c>
+      <c r="H107">
+        <v>881.1</v>
+      </c>
+      <c r="I107">
+        <v>82.7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>278</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108">
+        <v>991.9</v>
+      </c>
+      <c r="C108">
+        <v>86.42</v>
+      </c>
+      <c r="D108">
+        <v>980.9</v>
+      </c>
+      <c r="E108">
+        <v>85.56</v>
+      </c>
+      <c r="F108">
+        <v>970.2</v>
+      </c>
+      <c r="G108">
+        <v>88.94</v>
+      </c>
+      <c r="H108">
+        <v>970</v>
+      </c>
+      <c r="I108">
+        <v>89.65</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>279</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>926</v>
+      </c>
+      <c r="C109">
+        <v>84.67</v>
+      </c>
+      <c r="D109">
+        <v>935</v>
+      </c>
+      <c r="E109">
+        <v>87.3</v>
+      </c>
+      <c r="F109">
+        <v>908.9</v>
+      </c>
+      <c r="G109">
+        <v>84.06</v>
+      </c>
+      <c r="H109">
+        <v>914.1</v>
+      </c>
+      <c r="I109">
+        <v>80.680000000000007</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>280</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110">
+        <v>833.6</v>
+      </c>
+      <c r="C110">
+        <v>86.42</v>
+      </c>
+      <c r="D110">
+        <v>824.5</v>
+      </c>
+      <c r="E110">
+        <v>85.55</v>
+      </c>
+      <c r="F110">
+        <v>846.5</v>
+      </c>
+      <c r="G110">
+        <v>88.1</v>
+      </c>
+      <c r="H110">
+        <v>851.2</v>
+      </c>
+      <c r="I110">
+        <v>85.01</v>
+      </c>
+      <c r="J110" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>281</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111">
+        <v>910.5</v>
+      </c>
+      <c r="C111">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="D111">
+        <v>864.8</v>
+      </c>
+      <c r="E111">
+        <v>86.29</v>
+      </c>
+      <c r="F111">
+        <v>875.3</v>
+      </c>
+      <c r="G111">
+        <v>85.87</v>
+      </c>
+      <c r="H111">
+        <v>901</v>
+      </c>
+      <c r="I111">
+        <v>77.31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>282</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>772.2</v>
+      </c>
+      <c r="C112">
+        <v>88.66</v>
+      </c>
+      <c r="D112">
+        <v>746.6</v>
+      </c>
+      <c r="E112">
+        <v>85.24</v>
+      </c>
+      <c r="F112">
+        <v>759.9</v>
+      </c>
+      <c r="G112">
+        <v>80.760000000000005</v>
+      </c>
+      <c r="H112">
+        <v>774.7</v>
+      </c>
+      <c r="I112">
+        <v>87.48</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>283</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>938</v>
+      </c>
+      <c r="C113">
+        <v>89.63</v>
+      </c>
+      <c r="D113">
+        <v>870</v>
+      </c>
+      <c r="E113">
+        <v>80.47</v>
+      </c>
+      <c r="F113">
+        <v>888.2</v>
+      </c>
+      <c r="G113">
+        <v>86</v>
+      </c>
+      <c r="H113">
+        <v>948.3</v>
+      </c>
+      <c r="I113">
+        <v>86.01</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>284</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>912</v>
+      </c>
+      <c r="C114">
+        <v>89.56</v>
+      </c>
+      <c r="D114">
+        <v>874.7</v>
+      </c>
+      <c r="E114">
+        <v>86.46</v>
+      </c>
+      <c r="F114">
+        <v>903.4</v>
+      </c>
+      <c r="G114">
+        <v>88.29</v>
+      </c>
+      <c r="H114">
+        <v>894.1</v>
+      </c>
+      <c r="I114">
+        <v>81.38</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>285</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>904.3</v>
+      </c>
+      <c r="C115">
+        <v>84.42</v>
+      </c>
+      <c r="D115">
+        <v>876</v>
+      </c>
+      <c r="E115">
+        <v>79.739999999999995</v>
+      </c>
+      <c r="F115">
+        <v>865.7</v>
+      </c>
+      <c r="G115">
+        <v>76.569999999999993</v>
+      </c>
+      <c r="H115">
+        <v>898.1</v>
+      </c>
+      <c r="I115">
+        <v>81.42</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>286</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>972.1</v>
+      </c>
+      <c r="C116">
+        <v>89.06</v>
+      </c>
+      <c r="D116">
+        <v>952.9</v>
+      </c>
+      <c r="E116">
+        <v>80.58</v>
+      </c>
+      <c r="F116">
+        <v>932.3</v>
+      </c>
+      <c r="G116">
+        <v>85.94</v>
+      </c>
+      <c r="H116">
+        <v>959.3</v>
+      </c>
+      <c r="I116">
+        <v>85.22</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>287</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>942.2</v>
+      </c>
+      <c r="C117">
+        <v>86.11</v>
+      </c>
+      <c r="D117">
+        <v>868.1</v>
+      </c>
+      <c r="E117">
+        <v>79.650000000000006</v>
+      </c>
+      <c r="F117">
+        <v>858.8</v>
+      </c>
+      <c r="G117">
+        <v>77.36</v>
+      </c>
+      <c r="H117">
+        <v>953.4</v>
+      </c>
+      <c r="I117">
+        <v>86.87</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>288</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>976.1</v>
+      </c>
+      <c r="C118">
+        <v>89.06</v>
+      </c>
+      <c r="D118">
+        <v>927.1</v>
+      </c>
+      <c r="E118">
+        <v>87.16</v>
+      </c>
+      <c r="F118">
+        <v>902</v>
+      </c>
+      <c r="G118">
+        <v>89.49</v>
+      </c>
+      <c r="H118">
+        <v>958</v>
+      </c>
+      <c r="I118">
+        <v>89.52</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>289</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>966.5</v>
+      </c>
+      <c r="C119">
+        <v>85.91</v>
+      </c>
+      <c r="D119">
+        <v>941.2</v>
+      </c>
+      <c r="E119">
+        <v>87.08</v>
+      </c>
+      <c r="F119">
+        <v>923.1</v>
+      </c>
+      <c r="G119">
+        <v>89.13</v>
+      </c>
+      <c r="H119">
+        <v>972.5</v>
+      </c>
+      <c r="I119">
+        <v>85.16</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>290</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>862</v>
+      </c>
+      <c r="C120">
+        <v>89.8</v>
+      </c>
+      <c r="D120">
+        <v>799.5</v>
+      </c>
+      <c r="E120">
+        <v>85.48</v>
+      </c>
+      <c r="F120">
+        <v>801.1</v>
+      </c>
+      <c r="G120">
+        <v>85.85</v>
+      </c>
+      <c r="H120">
+        <v>858.8</v>
+      </c>
+      <c r="I120">
+        <v>87.6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>291</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>969.3</v>
+      </c>
+      <c r="C121">
+        <v>82.05</v>
+      </c>
+      <c r="D121">
+        <v>891.1</v>
+      </c>
+      <c r="E121">
+        <v>87.17</v>
+      </c>
+      <c r="F121">
+        <v>887.4</v>
+      </c>
+      <c r="G121">
+        <v>84.96</v>
+      </c>
+      <c r="H121">
+        <v>960.7</v>
+      </c>
+      <c r="I121">
+        <v>85.7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>292</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>879</v>
+      </c>
+      <c r="C122">
+        <v>87.26</v>
+      </c>
+      <c r="D122">
+        <v>863.8</v>
+      </c>
+      <c r="E122">
+        <v>86.28</v>
+      </c>
+      <c r="F122">
+        <v>912.4</v>
+      </c>
+      <c r="G122">
+        <v>83.2</v>
+      </c>
+      <c r="H122">
+        <v>904.2</v>
+      </c>
+      <c r="I122">
+        <v>88.73</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>293</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>984.8</v>
+      </c>
+      <c r="C123">
+        <v>80.06</v>
+      </c>
+      <c r="D123">
+        <v>952.6</v>
+      </c>
+      <c r="E123">
+        <v>85.79</v>
+      </c>
+      <c r="F123">
+        <v>950</v>
+      </c>
+      <c r="G123">
+        <v>89.52</v>
+      </c>
+      <c r="H123">
+        <v>1025.0999999999999</v>
+      </c>
+      <c r="I123">
+        <v>82.38</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>294</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>892</v>
+      </c>
+      <c r="C124">
+        <v>89.87</v>
+      </c>
+      <c r="D124">
+        <v>815.1</v>
+      </c>
+      <c r="E124">
+        <v>78.97</v>
+      </c>
+      <c r="F124">
+        <v>830.3</v>
+      </c>
+      <c r="G124">
+        <v>84.19</v>
+      </c>
+      <c r="H124">
+        <v>900.3</v>
+      </c>
+      <c r="I124">
+        <v>88.47</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>295</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>818.3</v>
+      </c>
+      <c r="C125">
+        <v>88.46</v>
+      </c>
+      <c r="D125">
+        <v>784.7</v>
+      </c>
+      <c r="E125">
+        <v>83.71</v>
+      </c>
+      <c r="F125">
+        <v>773.2</v>
+      </c>
+      <c r="G125">
+        <v>84.81</v>
+      </c>
+      <c r="H125">
+        <v>814.1</v>
+      </c>
+      <c r="I125">
+        <v>77.23</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>296</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>938.9</v>
+      </c>
+      <c r="C126">
+        <v>82.1</v>
+      </c>
+      <c r="D126">
+        <v>927.4</v>
+      </c>
+      <c r="E126">
+        <v>88.33</v>
+      </c>
+      <c r="F126">
+        <v>919.2</v>
+      </c>
+      <c r="G126">
+        <v>88.94</v>
+      </c>
+      <c r="H126">
+        <v>935.5</v>
+      </c>
+      <c r="I126">
+        <v>81.010000000000005</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>297</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>1023.4</v>
+      </c>
+      <c r="C127">
+        <v>85.35</v>
+      </c>
+      <c r="D127">
+        <v>973.6</v>
+      </c>
+      <c r="E127">
+        <v>86.7</v>
+      </c>
+      <c r="F127">
+        <v>965.5</v>
+      </c>
+      <c r="G127">
+        <v>86.85</v>
+      </c>
+      <c r="H127">
+        <v>990.4</v>
+      </c>
+      <c r="I127">
+        <v>86.01</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>298</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>928.2</v>
+      </c>
+      <c r="C128">
+        <v>88.77</v>
+      </c>
+      <c r="D128">
+        <v>938.1</v>
+      </c>
+      <c r="E128">
+        <v>84.62</v>
+      </c>
+      <c r="F128">
+        <v>906</v>
+      </c>
+      <c r="G128">
+        <v>89.75</v>
+      </c>
+      <c r="H128">
+        <v>925.6</v>
+      </c>
+      <c r="I128">
+        <v>83.67</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>299</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>942.5</v>
+      </c>
+      <c r="C129">
+        <v>88.05</v>
+      </c>
+      <c r="D129">
+        <v>878.1</v>
+      </c>
+      <c r="E129">
+        <v>89.22</v>
+      </c>
+      <c r="F129">
+        <v>896.9</v>
+      </c>
+      <c r="G129">
+        <v>87.44</v>
+      </c>
+      <c r="H129">
+        <v>912.8</v>
+      </c>
+      <c r="I129">
+        <v>85.48</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>300</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>893.8</v>
+      </c>
+      <c r="C130">
+        <v>86.41</v>
+      </c>
+      <c r="D130">
+        <v>801.8</v>
+      </c>
+      <c r="E130">
+        <v>83.12</v>
+      </c>
+      <c r="F130">
+        <v>790.1</v>
+      </c>
+      <c r="G130">
+        <v>88.98</v>
+      </c>
+      <c r="H130">
+        <v>880</v>
+      </c>
+      <c r="I130">
+        <v>81.37</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>301</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>864.1</v>
+      </c>
+      <c r="C131">
+        <v>84.42</v>
+      </c>
+      <c r="D131">
+        <v>773.6</v>
+      </c>
+      <c r="E131">
+        <v>87.78</v>
+      </c>
+      <c r="F131">
+        <v>833.7</v>
+      </c>
+      <c r="G131">
+        <v>87.59</v>
+      </c>
+      <c r="H131">
+        <v>860.2</v>
+      </c>
+      <c r="I131">
+        <v>85.93</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>302</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>881.8</v>
+      </c>
+      <c r="C132">
+        <v>86.36</v>
+      </c>
+      <c r="D132">
+        <v>812.4</v>
+      </c>
+      <c r="E132">
+        <v>88.31</v>
+      </c>
+      <c r="F132">
+        <v>828.7</v>
+      </c>
+      <c r="G132">
+        <v>83.9</v>
+      </c>
+      <c r="H132">
+        <v>890</v>
+      </c>
+      <c r="I132">
+        <v>89.87</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>303</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>974.1</v>
+      </c>
+      <c r="C133">
+        <v>89.06</v>
+      </c>
+      <c r="D133">
+        <v>909.7</v>
+      </c>
+      <c r="E133">
+        <v>84.83</v>
+      </c>
+      <c r="F133">
+        <v>910.1</v>
+      </c>
+      <c r="G133">
+        <v>84.58</v>
+      </c>
+      <c r="H133">
+        <v>978</v>
+      </c>
+      <c r="I133">
+        <v>89.65</v>
+      </c>
+      <c r="J133" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>304</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>878.7</v>
+      </c>
+      <c r="C134">
+        <v>82.94</v>
+      </c>
+      <c r="D134">
+        <v>792.2</v>
+      </c>
+      <c r="E134">
+        <v>88.84</v>
+      </c>
+      <c r="F134">
+        <v>792.2</v>
+      </c>
+      <c r="G134">
+        <v>88.84</v>
+      </c>
+      <c r="H134">
+        <v>857.6</v>
+      </c>
+      <c r="I134">
+        <v>83.44</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>305</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>980.2</v>
+      </c>
+      <c r="C135">
+        <v>88.71</v>
+      </c>
+      <c r="D135">
+        <v>872.1</v>
+      </c>
+      <c r="E135">
+        <v>89.08</v>
+      </c>
+      <c r="F135">
+        <v>870.1</v>
+      </c>
+      <c r="G135">
+        <v>89.34</v>
+      </c>
+      <c r="H135">
+        <v>967.2</v>
+      </c>
+      <c r="I135">
+        <v>87.16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>306</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>911.8</v>
+      </c>
+      <c r="C136">
+        <v>83.51</v>
+      </c>
+      <c r="D136">
+        <v>842.7</v>
+      </c>
+      <c r="E136">
+        <v>87.69</v>
+      </c>
+      <c r="F136">
+        <v>869</v>
+      </c>
+      <c r="G136">
+        <v>89.87</v>
+      </c>
+      <c r="H136">
+        <v>903.2</v>
+      </c>
+      <c r="I136">
+        <v>87.02</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>307</v>
+      </c>
+      <c r="B137">
+        <v>852.1</v>
+      </c>
+      <c r="C137">
+        <v>83.13</v>
+      </c>
+      <c r="D137">
+        <v>816.4</v>
+      </c>
+      <c r="E137">
+        <v>75.39</v>
+      </c>
+      <c r="F137">
+        <v>814.6</v>
+      </c>
+      <c r="G137">
+        <v>73.75</v>
+      </c>
+      <c r="H137">
+        <v>826.2</v>
+      </c>
+      <c r="I137">
+        <v>81.93</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>308</v>
+      </c>
+      <c r="B138">
+        <v>958.1</v>
+      </c>
+      <c r="C138">
+        <v>89.04</v>
+      </c>
+      <c r="D138">
+        <v>989.7</v>
+      </c>
+      <c r="E138">
+        <v>86.64</v>
+      </c>
+      <c r="F138">
+        <v>964.8</v>
+      </c>
+      <c r="G138">
+        <v>87.62</v>
+      </c>
+      <c r="H138">
+        <v>958.6</v>
+      </c>
+      <c r="I138">
+        <v>87.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>